<commit_message>
made changes to package for deployment
</commit_message>
<xml_diff>
--- a/jobs.xlsx
+++ b/jobs.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="56">
   <si>
     <t>username</t>
   </si>
@@ -151,15 +151,9 @@
     <t xml:space="preserve">   </t>
   </si>
   <si>
-    <t>afdfdfsdfsdfv</t>
-  </si>
-  <si>
     <t>abcd</t>
   </si>
   <si>
-    <t>..;;:</t>
-  </si>
-  <si>
     <t>anand122@gmail.coma</t>
   </si>
   <si>
@@ -185,6 +179,12 @@
   </si>
   <si>
     <t>&lt;&gt;,.</t>
+  </si>
+  <si>
+    <t>afafa</t>
+  </si>
+  <si>
+    <t>aadsad</t>
   </si>
 </sst>
 </file>
@@ -531,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -574,29 +574,9 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" t="s">
-        <v>44</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
@@ -618,7 +598,7 @@
         <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H3">
         <v>20000</v>
@@ -844,54 +824,54 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="F13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>20000</v>
+        <v>50</v>
+      </c>
+      <c r="G13" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="F14" t="s">
-        <v>52</v>
-      </c>
-      <c r="G14" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14" t="s">
-        <v>54</v>
+        <v>13</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>20000</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -934,7 +914,7 @@
         <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F16" t="s">
         <v>13</v>
@@ -1228,6 +1208,9 @@
     </row>
     <row r="28" spans="1:8">
       <c r="B28" s="1"/>
+      <c r="D28" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="29" spans="1:8">
       <c r="B29" s="1"/>
@@ -1441,31 +1424,30 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B10" r:id="rId8"/>
-    <hyperlink ref="B11" r:id="rId9"/>
-    <hyperlink ref="B12" r:id="rId10"/>
-    <hyperlink ref="B13" r:id="rId11"/>
-    <hyperlink ref="B15" r:id="rId12"/>
-    <hyperlink ref="B16" r:id="rId13"/>
-    <hyperlink ref="B17" r:id="rId14"/>
-    <hyperlink ref="B18" r:id="rId15"/>
-    <hyperlink ref="B19" r:id="rId16"/>
-    <hyperlink ref="B20" r:id="rId17"/>
-    <hyperlink ref="B21" r:id="rId18"/>
-    <hyperlink ref="B22" r:id="rId19"/>
-    <hyperlink ref="B23" r:id="rId20"/>
-    <hyperlink ref="B24" r:id="rId21"/>
-    <hyperlink ref="B25" r:id="rId22"/>
-    <hyperlink ref="B26" r:id="rId23"/>
-    <hyperlink ref="B27" r:id="rId24"/>
-    <hyperlink ref="B14" r:id="rId25"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B6" r:id="rId4"/>
+    <hyperlink ref="B7" r:id="rId5"/>
+    <hyperlink ref="B8" r:id="rId6"/>
+    <hyperlink ref="B10" r:id="rId7"/>
+    <hyperlink ref="B11" r:id="rId8"/>
+    <hyperlink ref="B12" r:id="rId9"/>
+    <hyperlink ref="B15" r:id="rId10"/>
+    <hyperlink ref="B16" r:id="rId11"/>
+    <hyperlink ref="B17" r:id="rId12"/>
+    <hyperlink ref="B18" r:id="rId13"/>
+    <hyperlink ref="B19" r:id="rId14"/>
+    <hyperlink ref="B20" r:id="rId15"/>
+    <hyperlink ref="B21" r:id="rId16"/>
+    <hyperlink ref="B22" r:id="rId17"/>
+    <hyperlink ref="B23" r:id="rId18"/>
+    <hyperlink ref="B24" r:id="rId19"/>
+    <hyperlink ref="B25" r:id="rId20"/>
+    <hyperlink ref="B26" r:id="rId21"/>
+    <hyperlink ref="B27" r:id="rId22"/>
+    <hyperlink ref="B13" r:id="rId23"/>
+    <hyperlink ref="B14" r:id="rId24"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>